<commit_message>
Budget update and papers
</commit_message>
<xml_diff>
--- a/Mazilu Budget.xlsx
+++ b/Mazilu Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwolf\Documents\Dartmouth\Research\Foosball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA71EAE0-C14B-433A-ADC9-5AB87B0CAEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E276905-EC74-42BC-B94E-10AFB8505BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28305" yWindow="480" windowWidth="13800" windowHeight="7095" xr2:uid="{C3F4C09E-6B7B-404A-9E2E-D54D4B818B55}"/>
+    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{C3F4C09E-6B7B-404A-9E2E-D54D4B818B55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Remaining Linear Components</t>
+  </si>
+  <si>
+    <t>#3-48 Screws and Nuts</t>
+  </si>
+  <si>
+    <t>PJRC</t>
+  </si>
+  <si>
+    <t>Teensy 4.1s</t>
   </si>
 </sst>
 </file>
@@ -457,12 +466,13 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -499,7 +509,7 @@
       </c>
       <c r="F2" s="1">
         <f>10000-SUM(B2:B14)</f>
-        <v>864.90000000000146</v>
+        <v>747.70000000000073</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -626,10 +636,32 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>20.02</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44785</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <v>97.18</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44785</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>

</xml_diff>